<commit_message>
UAT Pre-commit: Fixing many bugs, adding signup process & password reset
</commit_message>
<xml_diff>
--- a/IndustrialParamedics/Equipment_Template.xlsx
+++ b/IndustrialParamedics/Equipment_Template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/i843286/Dropbox/Consulting/Projects &amp; Clients/IPS/industrial_mobile/IndustrialParamedics/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/i843286/Projects/IPS/industrial_mobile/IndustrialParamedics/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="22260" yWindow="1560" windowWidth="27640" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="1040" yWindow="6180" windowWidth="27640" windowHeight="16880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,12 +24,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>Job Number:</t>
-  </si>
-  <si>
-    <t>Customer / Clinic:</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -81,9 +78,6 @@
     <t>Contact phone number</t>
   </si>
   <si>
-    <t>Next shift change date</t>
-  </si>
-  <si>
     <t>Explanation:</t>
   </si>
   <si>
@@ -105,31 +99,58 @@
     <t>Incident #:</t>
   </si>
   <si>
-    <t>%EquipmentForm.Name</t>
-  </si>
-  <si>
-    <t>%EquipmentForm.Date</t>
-  </si>
-  <si>
-    <t>%EquipmentForm.Phone</t>
-  </si>
-  <si>
-    <t>Equipment request Form</t>
-  </si>
-  <si>
-    <t>Title:</t>
-  </si>
-  <si>
-    <t>%EquipmentForm.Title</t>
-  </si>
-  <si>
-    <t>%EquipmentForm.Note</t>
-  </si>
-  <si>
-    <t>%EquipmentForm.Customer</t>
-  </si>
-  <si>
-    <t>%EquipmentForm.Job</t>
+    <t>Service Request Sheet</t>
+  </si>
+  <si>
+    <t>Incident Report #:</t>
+  </si>
+  <si>
+    <t>Vehicle Type:</t>
+  </si>
+  <si>
+    <t>Fuel Type:</t>
+  </si>
+  <si>
+    <t>Client Name:</t>
+  </si>
+  <si>
+    <t>Unit #:</t>
+  </si>
+  <si>
+    <t>MTC #:</t>
+  </si>
+  <si>
+    <t>%VehicleForm.Job</t>
+  </si>
+  <si>
+    <t>%VehicleForm.Customer</t>
+  </si>
+  <si>
+    <t>%VehicleForm.IncidentNum</t>
+  </si>
+  <si>
+    <t>%VehicleForm.Name</t>
+  </si>
+  <si>
+    <t>%VehicleForm.Date</t>
+  </si>
+  <si>
+    <t>%VehicleForm.Phone</t>
+  </si>
+  <si>
+    <t>%VehicleForm.VehicleType</t>
+  </si>
+  <si>
+    <t>%VehicleForm.FuelType</t>
+  </si>
+  <si>
+    <t>%VehicleForm.Unit</t>
+  </si>
+  <si>
+    <t>%VehicleForm.MTC</t>
+  </si>
+  <si>
+    <t>%VehicleForm.Note</t>
   </si>
 </sst>
 </file>
@@ -139,21 +160,6 @@
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -213,6 +219,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -246,17 +267,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
@@ -327,95 +337,113 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -442,7 +470,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>333376</xdr:colOff>
+      <xdr:colOff>41276</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>111125</xdr:rowOff>
     </xdr:to>
@@ -737,100 +765,110 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:E11"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="7" max="7" width="21.5" customWidth="1"/>
     <col min="9" max="9" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="I1" s="34"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H1" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="39"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" s="34"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G2" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="39"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="3"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G3" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="39"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" ht="24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="5" t="s">
-        <v>21</v>
-      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>4</v>
+    <row r="6" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="27"/>
+      <c r="M6" s="27"/>
+      <c r="N6" s="27"/>
+      <c r="O6" s="27"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -841,8 +879,10 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -852,297 +892,309 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9" t="s">
+      <c r="G10" s="4"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="4"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" s="1"/>
+      <c r="B13" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="8"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="8"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="35" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="35"/>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="35" t="s">
-        <v>19</v>
-      </c>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="1"/>
-      <c r="B12" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="35"/>
-      <c r="C13" s="35"/>
+      <c r="C13" s="6"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="1"/>
-      <c r="B14" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="29"/>
+      <c r="C14" s="29"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="10" t="s">
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15" s="1"/>
+      <c r="B15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="37"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="37"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="37"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="37"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="37"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="37"/>
+      <c r="G21" s="37"/>
+      <c r="H21" s="37"/>
+      <c r="I21" s="37"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="28"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="26"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="7"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="I14" s="1"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="32" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="32"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="32"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="12" t="s">
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="10"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="32"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="H24" s="32"/>
+      <c r="I24" s="33"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="12"/>
+      <c r="B25" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="32"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="39" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" s="39"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="39"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="39"/>
-      <c r="I17" s="39"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="39" t="s">
-        <v>2</v>
-      </c>
-      <c r="B18" s="39"/>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="39"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="39"/>
-      <c r="I18" s="39"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="39" t="s">
-        <v>2</v>
-      </c>
-      <c r="B19" s="39"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="39"/>
-      <c r="I19" s="39"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="39" t="s">
-        <v>2</v>
-      </c>
-      <c r="B20" s="39"/>
-      <c r="C20" s="39"/>
-      <c r="D20" s="39"/>
-      <c r="E20" s="39"/>
-      <c r="F20" s="39"/>
-      <c r="G20" s="39"/>
-      <c r="H20" s="39"/>
-      <c r="I20" s="39"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="13"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15" t="s">
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="16"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="40" t="s">
-        <v>2</v>
-      </c>
-      <c r="B22" s="37"/>
-      <c r="C22" s="37"/>
-      <c r="D22" s="37"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="36" t="s">
-        <v>2</v>
-      </c>
-      <c r="H22" s="37"/>
-      <c r="I22" s="38"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="18"/>
-      <c r="B23" s="19" t="s">
+      <c r="I25" s="15"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="20" t="s">
+      <c r="B26" s="17"/>
+      <c r="C26" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" s="32"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="I23" s="21"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="22" t="s">
+      <c r="H26" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="I26" s="33"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="19"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="20"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="21"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="23"/>
-      <c r="C24" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" s="37"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="H24" s="36" t="s">
-        <v>2</v>
-      </c>
-      <c r="I24" s="38"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="25"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" s="26"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="27"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="B26" s="36" t="s">
-        <v>2</v>
-      </c>
-      <c r="C26" s="37"/>
-      <c r="D26" s="37"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="27"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="29"/>
-      <c r="B27" s="30"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="30"/>
-      <c r="G27" s="30"/>
-      <c r="H27" s="30"/>
-      <c r="I27" s="31"/>
+      <c r="B28" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="21"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="23"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="24"/>
+      <c r="H29" s="24"/>
+      <c r="I29" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="A17:I17"/>
-    <mergeCell ref="A18:I18"/>
-    <mergeCell ref="A19:I19"/>
-    <mergeCell ref="A20:I20"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="B15:I15"/>
-    <mergeCell ref="B16:I16"/>
+  <mergeCells count="18">
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="B21:I21"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="H2:I2"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="A6:I6"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="B20:I20"/>
+    <mergeCell ref="B17:I17"/>
+    <mergeCell ref="B18:I18"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A9" r:id="rId1" display="mailto:billings@ipsems.com"/>
+    <hyperlink ref="A10" r:id="rId1" display="mailto:billings@ipsems.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>

</xml_diff>